<commit_message>
feat: update COVAC_tracker for DHIS2v 2.33, 2.34, 2.35
</commit_message>
<xml_diff>
--- a/metadata/COVAC_Tracker/COVAC_TRACKER_V1_DHIS2.33/reference.xlsx
+++ b/metadata/COVAC_Tracker/COVAC_TRACKER_V1_DHIS2.33/reference.xlsx
@@ -449,7 +449,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -481,7 +481,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC</v>
+        <v>V1.1.2</v>
       </c>
     </row>
     <row r="5">
@@ -489,7 +489,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>TRACKER</v>
+        <v>DHIS2.33.8-3c90b70</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +497,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>V1.1.2</v>
+        <v>20210406T115721</v>
       </c>
     </row>
     <row r="7">
@@ -505,7 +505,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC_TRACKER_COVAC_TRACKER_V1.1.2_DHIS2.33.8-3c90b70_20210318T130229</v>
+        <v>COVAC_TRACKER_V1.1.2_DHIS2.33.8-3c90b70_20210406T115721</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +582,7 @@
         <v>s2slttllN6D</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>sB1IHYu2xQT</v>
+        <v>First Name</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>sB1IHYu2xQT</v>
@@ -599,7 +599,7 @@
         <v>CbvQnJ9vOOd</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>ENRjVGxVL6l</v>
+        <v>Surname</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>ENRjVGxVL6l</v>
@@ -616,7 +616,7 @@
         <v>kbwzu78u3JT</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>oindugucx72</v>
+        <v>Sex</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>oindugucx72</v>
@@ -650,7 +650,7 @@
         <v>dSiYRbN6NKt</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>NI0QRzJvQ0k</v>
+        <v>Date of birth</v>
       </c>
       <c r="C8" s="4" t="str">
         <v>NI0QRzJvQ0k</v>
@@ -684,7 +684,7 @@
         <v>fWwyEWSOqKq</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Xhdn49gUd52</v>
+        <v>Home Address</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>Xhdn49gUd52</v>
@@ -1330,7 +1330,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVAC - Renal Disease</v>
+        <v>COVAC - Neurological/Neuromuscular</v>
       </c>
     </row>
     <row r="3">
@@ -1338,7 +1338,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVAC - Underlying condition</v>
+        <v>COVAC - Immunodeficiency</v>
       </c>
     </row>
     <row r="4">
@@ -1346,7 +1346,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVAC- Batch Number</v>
+        <v>COVAC - Renal Disease</v>
       </c>
     </row>
     <row r="5">
@@ -1354,7 +1354,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVAC - Pregnancy</v>
+        <v>COVAC - Multiple products used - Explain</v>
       </c>
     </row>
     <row r="6">
@@ -1362,7 +1362,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVAC - Dose Expiry Date</v>
+        <v>COVAC - Total doses</v>
       </c>
     </row>
     <row r="7">
@@ -1370,7 +1370,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAC - Total doses</v>
+        <v>COVAC - Underlying condition</v>
       </c>
     </row>
     <row r="8">
@@ -1378,7 +1378,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVAC - Dose Number</v>
+        <v>COVAC - Vaccine Name</v>
       </c>
     </row>
     <row r="9">
@@ -1386,7 +1386,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVAC - Cardiovascular Disease</v>
+        <v>COVAC - Last Dose</v>
       </c>
     </row>
     <row r="10">
@@ -1394,7 +1394,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVAC - Chronic Lung Disease</v>
+        <v>COVAC- Batch Number</v>
       </c>
     </row>
     <row r="11">
@@ -1402,7 +1402,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVAC - AEFIs present</v>
+        <v>COVAC - Allergic reaction after first dose</v>
       </c>
     </row>
     <row r="12">
@@ -1410,7 +1410,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVAC Suggested date for next dose</v>
+        <v>COVAC - Underlying condition Other</v>
       </c>
     </row>
     <row r="13">
@@ -1418,7 +1418,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVAC Previously infected with COVID</v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="14">
@@ -1426,7 +1426,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVAC - Neurological/Neuromuscular</v>
+        <v>COVAC - Pregnancy</v>
       </c>
     </row>
     <row r="15">
@@ -1434,7 +1434,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVAC - Immunodeficiency</v>
+        <v>COVAC - Dose Expiry Date</v>
       </c>
     </row>
     <row r="16">
@@ -1442,7 +1442,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>COVAC - Multiple products used - Explain</v>
+        <v>COVAC - Diabetes</v>
       </c>
     </row>
     <row r="17">
@@ -1450,7 +1450,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>COVAC - Vaccine Name</v>
+        <v>COVAC - Pregnancy gestation</v>
       </c>
     </row>
     <row r="18">
@@ -1458,7 +1458,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>COVAC - Last Dose</v>
+        <v>COVAC - Dose Number</v>
       </c>
     </row>
     <row r="19">
@@ -1466,7 +1466,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>COVAC - Allergic reaction after first dose</v>
+        <v>COVAC - Malignancy</v>
       </c>
     </row>
     <row r="20">
@@ -1474,7 +1474,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>COVAC - Underlying condition Other</v>
+        <v>COVAC - Cardiovascular Disease</v>
       </c>
     </row>
     <row r="21">
@@ -1482,7 +1482,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>COVAC - Diabetes</v>
+        <v>COVAC - Chronic Lung Disease</v>
       </c>
     </row>
     <row r="22">
@@ -1490,7 +1490,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>COVAC - Pregnancy gestation</v>
+        <v>COVAC - AEFIs present</v>
       </c>
     </row>
     <row r="23">
@@ -1498,7 +1498,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>COVAC - Malignancy</v>
+        <v>COVAC Suggested date for next dose</v>
       </c>
     </row>
     <row r="24">
@@ -1506,7 +1506,7 @@
         <v>COVAC - Covid-19 vaccination registry</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>COVAC - Vaccine Manufacturer</v>
+        <v>COVAC Previously infected with COVID</v>
       </c>
     </row>
   </sheetData>
@@ -4027,13 +4027,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="174.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
@@ -4092,10 +4092,10 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Date of birth is estimated</v>
+        <v>Date of birth</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v/>
+        <v>patinfo_ageonsetunit</v>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
@@ -4104,12 +4104,12 @@
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>Z1rLc1rVHK8</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Mobile phone number</v>
+        <v>Date of birth is estimated</v>
       </c>
       <c r="B5" s="5" t="str">
         <v/>
@@ -4121,15 +4121,15 @@
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>fctSQp5nAYl</v>
+        <v>Z1rLc1rVHK8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>National ID</v>
+        <v>First Name</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v/>
+        <v>first_name</v>
       </c>
       <c r="C6" s="4" t="str">
         <v/>
@@ -4138,23 +4138,108 @@
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Ewi7FUfcHAD</v>
+        <v>sB1IHYu2xQT</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
+        <v>Home Address</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v>patinfo_resadmin0</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E7" s="5" t="str">
+        <v>Xhdn49gUd52</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>Mobile phone number</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E8" s="4" t="str">
+        <v>fctSQp5nAYl</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="str">
+        <v>National ID</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="C9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E9" s="5" t="str">
+        <v>Ewi7FUfcHAD</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="str">
+        <v>Sex</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <v>patinfo_sex</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E10" s="4" t="str">
+        <v>oindugucx72</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="str">
+        <v>Surname</v>
+      </c>
+      <c r="B11" s="5" t="str">
+        <v>surname</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <v>The patient's surname (family name)</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="5" t="str">
+        <v>ENRjVGxVL6l</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="str">
         <v>Unique System Identifier (EPI)</v>
       </c>
-      <c r="B7" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C7" s="5" t="str">
+      <c r="B12" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C12" s="4" t="str">
         <v>System-generated unique ID following pattern: EPI prefix + value randomly generated (#####) - Customize the length depending on the target population of your implementation</v>
       </c>
-      <c r="D7" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E7" s="5" t="str">
+      <c r="D12" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="4" t="str">
         <v>KSr2yTdu1AI</v>
       </c>
     </row>
@@ -4197,7 +4282,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-03-16</v>
+        <v>2021-03-19</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yDuAzyqYABS</v>
@@ -4478,10 +4563,10 @@
         <v>Vaccination</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>Underlying Conditions</v>
+        <v>Vaccination information</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>COVAC - Renal Disease</v>
+        <v>COVAC - Vaccine Manufacturer</v>
       </c>
     </row>
     <row r="21">
@@ -4489,10 +4574,10 @@
         <v>Vaccination</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>Vaccination information</v>
+        <v>Underlying Conditions</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>COVAC - Vaccine Manufacturer</v>
+        <v>COVAC - Renal Disease</v>
       </c>
     </row>
     <row r="22">
@@ -4503,7 +4588,7 @@
         <v>Vaccination information</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>COVAC - Total doses</v>
+        <v>COVAC - Multiple products used - Explain</v>
       </c>
     </row>
     <row r="23">
@@ -4514,7 +4599,7 @@
         <v>Vaccination information</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>COVAC - Multiple products used - Explain</v>
+        <v>COVAC - Total doses</v>
       </c>
     </row>
     <row r="24">

</xml_diff>